<commit_message>
text answers and documentation
</commit_message>
<xml_diff>
--- a/1a.xlsx
+++ b/1a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Java\git\inf102f18-mandatory1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682DAE39-117B-41F9-B10C-DAE7385EB4FC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40760D2-62E2-4FE5-A3EC-6D0799AA4DC7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24744" windowHeight="7032" xr2:uid="{F30223E2-ECED-4509-A2AE-C948A6BDB1E6}"/>
   </bookViews>
@@ -1138,7 +1138,7 @@
   <dimension ref="B3:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>